<commit_message>
Update script to run Eig
</commit_message>
<xml_diff>
--- a/code/extraction_data_two-one_left.xlsx
+++ b/code/extraction_data_two-one_left.xlsx
@@ -56,2308 +56,2308 @@
   <dimension ref="A1:N52"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="true"/>
-    <col min="2" max="2" width="14.7109375" customWidth="true"/>
-    <col min="3" max="3" width="15.7109375" customWidth="true"/>
-    <col min="4" max="4" width="14.7109375" customWidth="true"/>
+    <col min="1" max="1" width="14.42578125" customWidth="true"/>
+    <col min="2" max="2" width="15.42578125" customWidth="true"/>
+    <col min="3" max="3" width="15.42578125" customWidth="true"/>
+    <col min="4" max="4" width="15.42578125" customWidth="true"/>
     <col min="5" max="5" width="14.42578125" customWidth="true"/>
-    <col min="6" max="6" width="15.42578125" customWidth="true"/>
+    <col min="6" max="6" width="14.7109375" customWidth="true"/>
     <col min="7" max="7" width="14.42578125" customWidth="true"/>
-    <col min="8" max="8" width="14.42578125" customWidth="true"/>
+    <col min="8" max="8" width="14.7109375" customWidth="true"/>
     <col min="9" max="9" width="14.7109375" customWidth="true"/>
-    <col min="10" max="10" width="14.42578125" customWidth="true"/>
-    <col min="11" max="11" width="14.42578125" customWidth="true"/>
-    <col min="12" max="12" width="15.42578125" customWidth="true"/>
-    <col min="13" max="13" width="13.7109375" customWidth="true"/>
-    <col min="14" max="14" width="14.42578125" customWidth="true"/>
+    <col min="10" max="10" width="14.7109375" customWidth="true"/>
+    <col min="11" max="11" width="15.42578125" customWidth="true"/>
+    <col min="12" max="12" width="14.42578125" customWidth="true"/>
+    <col min="13" max="13" width="14.42578125" customWidth="true"/>
+    <col min="14" max="14" width="14.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0">
-        <v>0.64511576677500004</v>
+        <v>-0.01555174970000002</v>
       </c>
       <c r="B1" s="0">
-        <v>0.71333442441999995</v>
+        <v>-0.19394141413999999</v>
       </c>
       <c r="C1" s="0">
-        <v>0.40568988675000006</v>
+        <v>-0.028794179085000038</v>
       </c>
       <c r="D1" s="0">
-        <v>0.31041164264999999</v>
+        <v>-0.068716616169999967</v>
       </c>
       <c r="E1" s="0">
-        <v>0.39470699712499996</v>
+        <v>0.032938436800000005</v>
       </c>
       <c r="F1" s="0">
-        <v>-0.22517923590000002</v>
+        <v>-0.52101315393500003</v>
       </c>
       <c r="G1" s="0">
-        <v>-0.03739413326499999</v>
+        <v>-0.65527746669999998</v>
       </c>
       <c r="H1" s="0">
-        <v>0.074083389694999988</v>
+        <v>-0.38168596715000003</v>
       </c>
       <c r="I1" s="0">
-        <v>0.13521829179</v>
+        <v>0.05419757950500001</v>
       </c>
       <c r="J1" s="0">
-        <v>-1.1196040291</v>
+        <v>-0.82928418195000009</v>
       </c>
       <c r="K1" s="0">
-        <v>0.73889913805000007</v>
+        <v>-0.34182829109500001</v>
       </c>
       <c r="L1" s="0">
-        <v>-0.50205722875000003</v>
+        <v>-0.34520613802</v>
       </c>
       <c r="M1" s="0">
-        <v>0.30266031277999994</v>
+        <v>-0.32798684099999997</v>
       </c>
       <c r="N1" s="0">
-        <v>-0.15049097219000004</v>
+        <v>0.34232256360000002</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>-0.23407386889999998</v>
+        <v>0.53120066341666661</v>
       </c>
       <c r="B2" s="0">
-        <v>0.19393864680000006</v>
+        <v>0.55311112562816667</v>
       </c>
       <c r="C2" s="0">
-        <v>0.68586243776</v>
+        <v>1.2225100804833333</v>
       </c>
       <c r="D2" s="0">
-        <v>0.86936176677999999</v>
+        <v>1.2294827021199333</v>
       </c>
       <c r="E2" s="0">
-        <v>0.46012630099999996</v>
+        <v>1.24186734016</v>
       </c>
       <c r="F2" s="0">
-        <v>0.0092971478500000204</v>
+        <v>0.97847538498333342</v>
       </c>
       <c r="G2" s="0">
-        <v>-0.22214162342999999</v>
+        <v>0.51787940728333326</v>
       </c>
       <c r="H2" s="0">
-        <v>-0.24697750165000004</v>
+        <v>0.15101081246666664</v>
       </c>
       <c r="I2" s="0">
-        <v>0.32615361613000005</v>
+        <v>0.79714347154999998</v>
       </c>
       <c r="J2" s="0">
-        <v>0.32605882091999994</v>
+        <v>0.034195112766666667</v>
       </c>
       <c r="K2" s="0">
-        <v>1.1641095403000001</v>
+        <v>1.8771839396333334</v>
       </c>
       <c r="L2" s="0">
-        <v>0.030882855250000008</v>
+        <v>0.68238967577233334</v>
       </c>
       <c r="M2" s="0">
-        <v>0.16141692227999993</v>
+        <v>0.62548152027999993</v>
       </c>
       <c r="N2" s="0">
-        <v>0.47729519085</v>
+        <v>0.98277844483333321</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>0.041857196706666655</v>
+        <v>-0.32079114894166672</v>
       </c>
       <c r="B3" s="0">
-        <v>-0.28032813760000003</v>
+        <v>-0.65764178303666676</v>
       </c>
       <c r="C3" s="0">
-        <v>-1.0428598201333334</v>
+        <v>-0.98918888758699997</v>
       </c>
       <c r="D3" s="0">
-        <v>-0.79283451285666673</v>
+        <v>-0.55598872860000004</v>
       </c>
       <c r="E3" s="0">
-        <v>-0.20193008856833333</v>
+        <v>-0.15372163057333335</v>
       </c>
       <c r="F3" s="0">
-        <v>-0.38375626212166669</v>
+        <v>-0.28770310188333337</v>
       </c>
       <c r="G3" s="0">
-        <v>-0.42459224780666671</v>
+        <v>-0.42955675584233338</v>
       </c>
       <c r="H3" s="0">
-        <v>-0.064244013983333348</v>
+        <v>-0.37388231720000004</v>
       </c>
       <c r="I3" s="0">
-        <v>0.041452001016666656</v>
+        <v>-0.29734816038166667</v>
       </c>
       <c r="J3" s="0">
-        <v>-1.1675622256</v>
+        <v>-0.77124590565000006</v>
       </c>
       <c r="K3" s="0">
-        <v>-0.67943481899666669</v>
+        <v>-1.2964387712266665</v>
       </c>
       <c r="L3" s="0">
-        <v>0.23774648556666664</v>
+        <v>0.016207337300000069</v>
       </c>
       <c r="M3" s="0">
-        <v>-0.59620603441833331</v>
+        <v>-0.75948422334999999</v>
       </c>
       <c r="N3" s="0">
-        <v>0.74114739758333337</v>
+        <v>0.76565065780666663</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>-0.32338462131000001</v>
+        <v>0.21399900354066664</v>
       </c>
       <c r="B4" s="0">
-        <v>-0.11789717124266666</v>
+        <v>-0.26654397168333333</v>
       </c>
       <c r="C4" s="0">
-        <v>-0.19512393808333331</v>
+        <v>0.083876188050333311</v>
       </c>
       <c r="D4" s="0">
-        <v>-1.0445642591533333</v>
+        <v>0.15476096173376669</v>
       </c>
       <c r="E4" s="0">
-        <v>-0.86260165063333338</v>
+        <v>-0.24066077571666664</v>
       </c>
       <c r="F4" s="0">
-        <v>-0.19732956306333332</v>
+        <v>-0.12811464592666663</v>
       </c>
       <c r="G4" s="0">
-        <v>0.056086134366666651</v>
+        <v>0.06990499791333335</v>
       </c>
       <c r="H4" s="0">
-        <v>0.53208305634999997</v>
+        <v>0.21253802094066668</v>
       </c>
       <c r="I4" s="0">
-        <v>-0.89375126989999998</v>
+        <v>0.32464144059</v>
       </c>
       <c r="J4" s="0">
-        <v>-0.95267871746666666</v>
+        <v>-0.37379983203333333</v>
       </c>
       <c r="K4" s="0">
-        <v>1.0794617708666667</v>
+        <v>0.53980697793333343</v>
       </c>
       <c r="L4" s="0">
-        <v>-0.4005744886</v>
+        <v>0.24307745701666664</v>
       </c>
       <c r="M4" s="0">
-        <v>0.3598890834666667</v>
+        <v>-0.2300070797499999</v>
       </c>
       <c r="N4" s="0">
-        <v>-0.36054775263333333</v>
+        <v>0.73407234077333328</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>-0.090778868003333332</v>
+        <v>-0.44259427168333337</v>
       </c>
       <c r="B5" s="0">
-        <v>-0.26783643506166666</v>
+        <v>-0.22298590358333337</v>
       </c>
       <c r="C5" s="0">
-        <v>-0.23543432107999998</v>
+        <v>-0.47195895323833337</v>
       </c>
       <c r="D5" s="0">
-        <v>-0.66707357206666673</v>
+        <v>-0.43682721596666668</v>
       </c>
       <c r="E5" s="0">
-        <v>-0.60025102279333331</v>
+        <v>-0.62290526498333332</v>
       </c>
       <c r="F5" s="0">
-        <v>-0.50841535361333334</v>
+        <v>-0.49149359245666668</v>
       </c>
       <c r="G5" s="0">
-        <v>-0.34911410449666669</v>
+        <v>-0.47979870345000003</v>
       </c>
       <c r="H5" s="0">
-        <v>-0.071938460169999996</v>
+        <v>-0.30986436712999998</v>
       </c>
       <c r="I5" s="0">
-        <v>-0.52268033161000005</v>
+        <v>-0.19636645376666667</v>
       </c>
       <c r="J5" s="0">
-        <v>-0.045205879003333338</v>
+        <v>-0.49259616651666666</v>
       </c>
       <c r="K5" s="0">
-        <v>-1.0904819025499999</v>
+        <v>-1.10929360334</v>
       </c>
       <c r="L5" s="0">
-        <v>0.012086787950000011</v>
+        <v>-0.46177328094666664</v>
       </c>
       <c r="M5" s="0">
-        <v>-0.50346117178333338</v>
+        <v>-0.87231323192333332</v>
       </c>
       <c r="N5" s="0">
-        <v>-0.89531450100666654</v>
+        <v>-0.8790669739000001</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>-0.40512334972666669</v>
+        <v>-0.16152488606666668</v>
       </c>
       <c r="B6" s="0">
-        <v>-0.086233208133333336</v>
+        <v>-0.58074046066666662</v>
       </c>
       <c r="C6" s="0">
-        <v>-0.53827297643333338</v>
+        <v>-0.63460750001666666</v>
       </c>
       <c r="D6" s="0">
-        <v>-0.69282721422666671</v>
+        <v>-1.0179953371000001</v>
       </c>
       <c r="E6" s="0">
-        <v>-0.53982203596666667</v>
+        <v>-0.88884102621666661</v>
       </c>
       <c r="F6" s="0">
-        <v>-0.47920167819999998</v>
+        <v>-0.68114505466666664</v>
       </c>
       <c r="G6" s="0">
-        <v>-0.23816344082999996</v>
+        <v>-0.30382277902166671</v>
       </c>
       <c r="H6" s="0">
-        <v>-0.2802901852666666</v>
+        <v>-0.13478221287666664</v>
       </c>
       <c r="I6" s="0">
-        <v>-0.54152897425000002</v>
+        <v>-0.16038059091166665</v>
       </c>
       <c r="J6" s="0">
-        <v>-0.69470623554333333</v>
+        <v>0.11043518411666653</v>
       </c>
       <c r="K6" s="0">
-        <v>-0.42668187273333336</v>
+        <v>-0.98735542925666664</v>
       </c>
       <c r="L6" s="0">
-        <v>-0.8737718137499999</v>
+        <v>-1.5158200231099999</v>
       </c>
       <c r="M6" s="0">
-        <v>-1.6216603730633334</v>
+        <v>-1.5935219320333334</v>
       </c>
       <c r="N6" s="0">
-        <v>-0.63272380343333334</v>
+        <v>-0.19326655244500007</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>0.10993474864999997</v>
+        <v>-0.28264771924999987</v>
       </c>
       <c r="B7" s="0">
-        <v>0.24754966001666662</v>
+        <v>-0.5467793961166667</v>
       </c>
       <c r="C7" s="0">
-        <v>0.2633765611333333</v>
+        <v>-0.20811554004999988</v>
       </c>
       <c r="D7" s="0">
-        <v>0.30779020395333334</v>
+        <v>-0.091400528699999983</v>
       </c>
       <c r="E7" s="0">
-        <v>-0.3137435875016667</v>
+        <v>-0.26657027078333329</v>
       </c>
       <c r="F7" s="0">
-        <v>-0.1131599784566667</v>
+        <v>-0.13786830723333321</v>
       </c>
       <c r="G7" s="0">
-        <v>0.01539052198333335</v>
+        <v>-0.26357441863666653</v>
       </c>
       <c r="H7" s="0">
-        <v>0.046254222136666578</v>
+        <v>0.16323046561166671</v>
       </c>
       <c r="I7" s="0">
-        <v>0.15203164743333331</v>
+        <v>0.12069962753333341</v>
       </c>
       <c r="J7" s="0">
-        <v>0.16937305341666664</v>
+        <v>-0.80633577443333326</v>
       </c>
       <c r="K7" s="0">
-        <v>-0.7077781701000001</v>
+        <v>-1.7042436295833334</v>
       </c>
       <c r="L7" s="0">
-        <v>0.32600290726666659</v>
+        <v>-0.31926034420333349</v>
       </c>
       <c r="M7" s="0">
-        <v>0.66935368006666662</v>
+        <v>-0.0095100037199998821</v>
       </c>
       <c r="N7" s="0">
-        <v>0.93330152330000005</v>
+        <v>-0.69708202524999996</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>0.38489090083333333</v>
+        <v>0.011874668799999974</v>
       </c>
       <c r="B8" s="0">
-        <v>-0.21611846063333334</v>
+        <v>-0.2211442857716667</v>
       </c>
       <c r="C8" s="0">
-        <v>-0.047795846650000001</v>
+        <v>-0.62079069080333327</v>
       </c>
       <c r="D8" s="0">
-        <v>0.56610931333333336</v>
+        <v>-0.11400574544999997</v>
       </c>
       <c r="E8" s="0">
-        <v>0.38524141812333335</v>
+        <v>-0.095237128966999984</v>
       </c>
       <c r="F8" s="0">
-        <v>0.5122306861</v>
+        <v>-0.23461706583666669</v>
       </c>
       <c r="G8" s="0">
-        <v>0.38571640333833324</v>
+        <v>-0.84943427730999987</v>
       </c>
       <c r="H8" s="0">
-        <v>0.28980958927200001</v>
+        <v>-0.80661691186666662</v>
       </c>
       <c r="I8" s="0">
-        <v>0.29670433103349997</v>
+        <v>-0.26041285696666666</v>
       </c>
       <c r="J8" s="0">
-        <v>1.2586894191866669</v>
+        <v>-0.80561437468333352</v>
       </c>
       <c r="K8" s="0">
-        <v>-1.4796975963000001</v>
+        <v>-0.79517414024999988</v>
       </c>
       <c r="L8" s="0">
-        <v>0.26839152196666666</v>
+        <v>-0.5915928066166668</v>
       </c>
       <c r="M8" s="0">
-        <v>0.15026188228333331</v>
+        <v>-0.11360654624333333</v>
       </c>
       <c r="N8" s="0">
-        <v>0.57417268435500002</v>
+        <v>0.49481057694999997</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>0.050324002566666637</v>
+        <v>-0.12015487178333337</v>
       </c>
       <c r="B9" s="0">
-        <v>-0.076003879533333346</v>
+        <v>-0.40474827495166665</v>
       </c>
       <c r="C9" s="0">
-        <v>-0.34955942926666672</v>
+        <v>-0.22668501528333337</v>
       </c>
       <c r="D9" s="0">
-        <v>0.23081340661666672</v>
+        <v>-0.2072464143433333</v>
       </c>
       <c r="E9" s="0">
-        <v>0.097344897800000024</v>
+        <v>-0.18545729904999997</v>
       </c>
       <c r="F9" s="0">
-        <v>-0.32778611748333331</v>
+        <v>-0.28080361896966666</v>
       </c>
       <c r="G9" s="0">
-        <v>0.24789632578166659</v>
+        <v>-0.41370833180000005</v>
       </c>
       <c r="H9" s="0">
-        <v>0.17730611458333331</v>
+        <v>-0.13679057194666666</v>
       </c>
       <c r="I9" s="0">
-        <v>0.17369271616999998</v>
+        <v>0.071192868449999946</v>
       </c>
       <c r="J9" s="0">
-        <v>0.35552557840666665</v>
+        <v>-0.21196828030000009</v>
       </c>
       <c r="K9" s="0">
-        <v>0.19218367233333344</v>
+        <v>-0.047308373372373314</v>
       </c>
       <c r="L9" s="0">
-        <v>0.63115082464999994</v>
+        <v>-0.69460357003333328</v>
       </c>
       <c r="M9" s="0">
-        <v>-0.39541251529666666</v>
+        <v>-0.91207773466999997</v>
       </c>
       <c r="N9" s="0">
-        <v>1.0298822557333331</v>
+        <v>0.28106500960666669</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>0.31989473178333333</v>
+        <v>0.020042722550000003</v>
       </c>
       <c r="B10" s="0">
-        <v>0.10148068862833337</v>
+        <v>0.27789582272999991</v>
       </c>
       <c r="C10" s="0">
-        <v>0.12977229479499999</v>
+        <v>0.44699190436666664</v>
       </c>
       <c r="D10" s="0">
-        <v>-0.53924824665999993</v>
+        <v>-0.07429853885000004</v>
       </c>
       <c r="E10" s="0">
-        <v>-0.46026747729999995</v>
+        <v>0.30477844023333334</v>
       </c>
       <c r="F10" s="0">
-        <v>-0.64466400514</v>
+        <v>0.16094390860666666</v>
       </c>
       <c r="G10" s="0">
-        <v>-0.046583613626666687</v>
+        <v>-0.022706951176666601</v>
       </c>
       <c r="H10" s="0">
-        <v>0.055418859633333345</v>
+        <v>0.44094004841666673</v>
       </c>
       <c r="I10" s="0">
-        <v>-0.026119087714433387</v>
+        <v>0.0056567436166666263</v>
       </c>
       <c r="J10" s="0">
-        <v>-0.21964056959166658</v>
+        <v>-0.092700054700000006</v>
       </c>
       <c r="K10" s="0">
-        <v>-1.0493182826333334</v>
+        <v>-0.099863995455833299</v>
       </c>
       <c r="L10" s="0">
-        <v>-0.0039315684833333142</v>
+        <v>-0.31991024551666669</v>
       </c>
       <c r="M10" s="0">
-        <v>-0.35020151335333327</v>
+        <v>-0.70127986606000003</v>
       </c>
       <c r="N10" s="0">
-        <v>-0.35661489355000003</v>
+        <v>-0.1445886705166668</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>-0.15851850430800002</v>
+        <v>0.11812487649666667</v>
       </c>
       <c r="B11" s="0">
-        <v>0.19548938739666666</v>
+        <v>0.13381325029999996</v>
       </c>
       <c r="C11" s="0">
-        <v>0.59737162627666662</v>
+        <v>0.19350924171</v>
       </c>
       <c r="D11" s="0">
-        <v>-0.16270894723733334</v>
+        <v>-0.22971334073050001</v>
       </c>
       <c r="E11" s="0">
-        <v>-0.05261191771999997</v>
+        <v>-0.19550169484999996</v>
       </c>
       <c r="F11" s="0">
-        <v>0.40870171189666665</v>
+        <v>-0.31497969858899999</v>
       </c>
       <c r="G11" s="0">
-        <v>0.50182928623666667</v>
+        <v>-0.36824206821666661</v>
       </c>
       <c r="H11" s="0">
-        <v>0.42751841233333332</v>
+        <v>-0.13650641947833336</v>
       </c>
       <c r="I11" s="0">
-        <v>0.47300689540000007</v>
+        <v>0.89021675976333325</v>
       </c>
       <c r="J11" s="0">
-        <v>0.25346512878333333</v>
+        <v>-0.33849539924999994</v>
       </c>
       <c r="K11" s="0">
-        <v>1.0734174908816667</v>
+        <v>0.79748566028333334</v>
       </c>
       <c r="L11" s="0">
-        <v>-0.063676067331666586</v>
+        <v>0.35283850903333341</v>
       </c>
       <c r="M11" s="0">
-        <v>0.6810654496166666</v>
+        <v>0.81714861996666666</v>
       </c>
       <c r="N11" s="0">
-        <v>0.031465686850000119</v>
+        <v>-0.40154899145</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>-0.53106226326666672</v>
+        <v>0.077822953700000003</v>
       </c>
       <c r="B12" s="0">
-        <v>-0.3788854676566667</v>
+        <v>-0.28001917344333338</v>
       </c>
       <c r="C12" s="0">
-        <v>-0.42614312852000003</v>
+        <v>-0.41015418894666666</v>
       </c>
       <c r="D12" s="0">
-        <v>-0.032348659049999992</v>
+        <v>-0.0059701699333333524</v>
       </c>
       <c r="E12" s="0">
-        <v>-0.17210144959999998</v>
+        <v>-0.07655175408333334</v>
       </c>
       <c r="F12" s="0">
-        <v>-0.094956448566666657</v>
+        <v>0.37693010070666666</v>
       </c>
       <c r="G12" s="0">
-        <v>-0.88346374478333334</v>
+        <v>-0.23852521067166665</v>
       </c>
       <c r="H12" s="0">
-        <v>-0.35109668256666671</v>
+        <v>-0.093328082438333321</v>
       </c>
       <c r="I12" s="0">
-        <v>0.22195989443333333</v>
+        <v>0.42538713021666663</v>
       </c>
       <c r="J12" s="0">
-        <v>0.55834759166333336</v>
+        <v>-0.38532233346666667</v>
       </c>
       <c r="K12" s="0">
-        <v>0.33943563269999999</v>
+        <v>-0.0038371776366667026</v>
       </c>
       <c r="L12" s="0">
-        <v>0.0034470782750000151</v>
+        <v>-0.020830305933333293</v>
       </c>
       <c r="M12" s="0">
-        <v>-0.74725238891666668</v>
+        <v>-0.54275791124999995</v>
       </c>
       <c r="N12" s="0">
-        <v>-0.19385803371666657</v>
+        <v>0.50942962273333348</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>-0.059555075616666661</v>
+        <v>0.048402926476666663</v>
       </c>
       <c r="B13" s="0">
-        <v>0.61343448977333348</v>
+        <v>0.18822546510000004</v>
       </c>
       <c r="C13" s="0">
-        <v>0.48112606051666668</v>
+        <v>0.30007718480333334</v>
       </c>
       <c r="D13" s="0">
-        <v>0.41944084256666658</v>
+        <v>0.080017382121666647</v>
       </c>
       <c r="E13" s="0">
-        <v>0.58316201555333336</v>
+        <v>0.1106939012866667</v>
       </c>
       <c r="F13" s="0">
-        <v>1.0809982549199999</v>
+        <v>0.11436547591666664</v>
       </c>
       <c r="G13" s="0">
-        <v>0.69065632033333335</v>
+        <v>0.37517688183333336</v>
       </c>
       <c r="H13" s="0">
-        <v>0.081042782495000007</v>
+        <v>-0.065813158199999999</v>
       </c>
       <c r="I13" s="0">
-        <v>0.25153970279666665</v>
+        <v>-0.11048628105166666</v>
       </c>
       <c r="J13" s="0">
-        <v>0.90110603918333332</v>
+        <v>0.051772390026666643</v>
       </c>
       <c r="K13" s="0">
-        <v>0.40312757619833328</v>
+        <v>0.32074700320333338</v>
       </c>
       <c r="L13" s="0">
-        <v>0.28507000698333335</v>
+        <v>0.018848281915000001</v>
       </c>
       <c r="M13" s="0">
-        <v>-0.62960303786999994</v>
+        <v>-1.1360009593</v>
       </c>
       <c r="N13" s="0">
-        <v>0.011708580000000024</v>
+        <v>-0.1444171127333333</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>-0.49262343617333332</v>
+        <v>-0.12457297988333332</v>
       </c>
       <c r="B14" s="0">
-        <v>0.0031301000566666404</v>
+        <v>0.33455328024999997</v>
       </c>
       <c r="C14" s="0">
-        <v>0.47385274128060034</v>
+        <v>0.044142867206666769</v>
       </c>
       <c r="D14" s="0">
-        <v>0.70851302326333332</v>
+        <v>-0.32080578322166675</v>
       </c>
       <c r="E14" s="0">
-        <v>0.66326815414999996</v>
+        <v>0.027909984614999994</v>
       </c>
       <c r="F14" s="0">
-        <v>0.22165874203566666</v>
+        <v>0.89346569142666654</v>
       </c>
       <c r="G14" s="0">
-        <v>0.32467599732333341</v>
+        <v>0.28506411182000002</v>
       </c>
       <c r="H14" s="0">
-        <v>0.093066212850000024</v>
+        <v>0.47714549050333338</v>
       </c>
       <c r="I14" s="0">
-        <v>0.37296272998333335</v>
+        <v>0.00356586339999998</v>
       </c>
       <c r="J14" s="0">
-        <v>0.21894331188000005</v>
+        <v>-0.30037242237166667</v>
       </c>
       <c r="K14" s="0">
-        <v>-0.02938045735</v>
+        <v>0.28894890841666676</v>
       </c>
       <c r="L14" s="0">
-        <v>-0.26596385596666672</v>
+        <v>0.088414573870000068</v>
       </c>
       <c r="M14" s="0">
-        <v>1.0213306969</v>
+        <v>0.3676913289</v>
       </c>
       <c r="N14" s="0">
-        <v>0.44165444420000005</v>
+        <v>0.88705347229666665</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>0.13473441371666667</v>
+        <v>-0.066630912963333316</v>
       </c>
       <c r="B15" s="0">
-        <v>0.22783246323333337</v>
+        <v>0.152613271775</v>
       </c>
       <c r="C15" s="0">
-        <v>0.41785781762133334</v>
+        <v>0.43360331712666667</v>
       </c>
       <c r="D15" s="0">
-        <v>0.0083985771883333671</v>
+        <v>0.38750731518333326</v>
       </c>
       <c r="E15" s="0">
-        <v>-0.068125639683333322</v>
+        <v>0.048228104973333324</v>
       </c>
       <c r="F15" s="0">
-        <v>0.066118797850000022</v>
+        <v>-0.12384684965000003</v>
       </c>
       <c r="G15" s="0">
-        <v>-0.32219420941666665</v>
+        <v>-0.25470208900833335</v>
       </c>
       <c r="H15" s="0">
-        <v>-0.14186380865000001</v>
+        <v>-0.036764807191666651</v>
       </c>
       <c r="I15" s="0">
-        <v>0.29037462656666663</v>
+        <v>0.088367025928333329</v>
       </c>
       <c r="J15" s="0">
-        <v>0.35670505451666668</v>
+        <v>0.26480051061666665</v>
       </c>
       <c r="K15" s="0">
-        <v>0.052101521964999981</v>
+        <v>0.17883141703899996</v>
       </c>
       <c r="L15" s="0">
-        <v>0.35202486746666661</v>
+        <v>0.022317388936666793</v>
       </c>
       <c r="M15" s="0">
-        <v>-0.31522881003999992</v>
+        <v>-0.049253899850000005</v>
       </c>
       <c r="N15" s="0">
-        <v>0.37127877965</v>
+        <v>0.04306020713333332</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>-0.65894368078333332</v>
+        <v>-0.41115522391666665</v>
       </c>
       <c r="B16" s="0">
-        <v>-0.68887835273166675</v>
+        <v>-0.72872832073333338</v>
       </c>
       <c r="C16" s="0">
-        <v>-0.49804862173333331</v>
+        <v>-0.083158143749999969</v>
       </c>
       <c r="D16" s="0">
-        <v>-0.29960355288233331</v>
+        <v>0.50831531011666664</v>
       </c>
       <c r="E16" s="0">
-        <v>-0.28016900652333337</v>
+        <v>0.44677129567333335</v>
       </c>
       <c r="F16" s="0">
-        <v>-0.38395389908499999</v>
+        <v>-0.30683861828333331</v>
       </c>
       <c r="G16" s="0">
-        <v>-0.060030908974666647</v>
+        <v>-0.44735190540666658</v>
       </c>
       <c r="H16" s="0">
-        <v>-0.37779370035000004</v>
+        <v>-0.33739371586333333</v>
       </c>
       <c r="I16" s="0">
-        <v>-0.77461109436666664</v>
+        <v>-0.22620092985333334</v>
       </c>
       <c r="J16" s="0">
-        <v>-0.080456974081666646</v>
+        <v>-0.28387927711333338</v>
       </c>
       <c r="K16" s="0">
-        <v>-1.6426531310499999</v>
+        <v>-0.30954241583333336</v>
       </c>
       <c r="L16" s="0">
-        <v>-2.5311054168333333</v>
+        <v>-0.91615827529999994</v>
       </c>
       <c r="M16" s="0">
-        <v>-2.0235793488000002</v>
+        <v>-1.2093128287499999</v>
       </c>
       <c r="N16" s="0">
-        <v>-2.3512035512999998</v>
+        <v>-1.5842760169166668</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>-1.4257737812</v>
+        <v>-0.76868913892700008</v>
       </c>
       <c r="B17" s="0">
-        <v>-0.77330877936666664</v>
+        <v>-0.59386690719333335</v>
       </c>
       <c r="C17" s="0">
-        <v>-0.62618116506666666</v>
+        <v>-0.48112001780000002</v>
       </c>
       <c r="D17" s="0">
-        <v>0.059389798533333371</v>
+        <v>-0.29349542483333335</v>
       </c>
       <c r="E17" s="0">
-        <v>0.27399047120999998</v>
+        <v>0.21973409123333332</v>
       </c>
       <c r="F17" s="0">
-        <v>-0.52231138069666661</v>
+        <v>-0.026406609900000017</v>
       </c>
       <c r="G17" s="0">
-        <v>-1.46152218</v>
+        <v>-0.16024129798366671</v>
       </c>
       <c r="H17" s="0">
-        <v>-1.1045753795666666</v>
+        <v>-0.18512956057000002</v>
       </c>
       <c r="I17" s="0">
-        <v>0.078577313350666672</v>
+        <v>0.20151292112566666</v>
       </c>
       <c r="J17" s="0">
-        <v>-1.2763858558700001</v>
+        <v>-1.7510317240143334</v>
       </c>
       <c r="K17" s="0">
-        <v>-0.3393536238</v>
+        <v>-0.19137783899999999</v>
       </c>
       <c r="L17" s="0">
-        <v>-2.0401980282999999</v>
+        <v>-0.51712668383333327</v>
       </c>
       <c r="M17" s="0">
-        <v>-0.89455599783666662</v>
+        <v>-0.4741356614333333</v>
       </c>
       <c r="N17" s="0">
-        <v>-1.1583807232333334</v>
+        <v>-0.34001798056333332</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>0.14027619191099999</v>
+        <v>0.083540368806666682</v>
       </c>
       <c r="B18" s="0">
-        <v>0.52763506756666667</v>
+        <v>0.3190007797333333</v>
       </c>
       <c r="C18" s="0">
-        <v>0.24220944719999998</v>
+        <v>0.56063261975666667</v>
       </c>
       <c r="D18" s="0">
-        <v>0.80172180829000006</v>
+        <v>0.80302907530000001</v>
       </c>
       <c r="E18" s="0">
-        <v>-0.14116222405666665</v>
+        <v>0.33750852162533335</v>
       </c>
       <c r="F18" s="0">
-        <v>0.077201284966666672</v>
+        <v>0.007306835296666675</v>
       </c>
       <c r="G18" s="0">
-        <v>0.016706315999999943</v>
+        <v>0.1005325071</v>
       </c>
       <c r="H18" s="0">
-        <v>0.30730734302333329</v>
+        <v>0.0044590571033333252</v>
       </c>
       <c r="I18" s="0">
-        <v>0.35345236478333336</v>
+        <v>0.3822654112633333</v>
       </c>
       <c r="J18" s="0">
-        <v>-0.57346931136666668</v>
+        <v>0.069916242500000003</v>
       </c>
       <c r="K18" s="0">
-        <v>0.1788348788666666</v>
+        <v>0.33536016349999997</v>
       </c>
       <c r="L18" s="0">
-        <v>0.7868660328999999</v>
+        <v>0.11318876929299999</v>
       </c>
       <c r="M18" s="0">
-        <v>-0.1283168713333333</v>
+        <v>0.44008467412666669</v>
       </c>
       <c r="N18" s="0">
-        <v>0.47390734651999999</v>
+        <v>-0.61917957926666656</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>0.61971470532166673</v>
+        <v>0.44085234376666665</v>
       </c>
       <c r="B19" s="0">
-        <v>0.60773934416999997</v>
+        <v>0.37705442513766663</v>
       </c>
       <c r="C19" s="0">
-        <v>0.55673937169499998</v>
+        <v>0.52843878061666671</v>
       </c>
       <c r="D19" s="0">
-        <v>-0.11908992375266667</v>
+        <v>0.30992696121999996</v>
       </c>
       <c r="E19" s="0">
-        <v>-0.42393645024333332</v>
+        <v>0.2375973987933333</v>
       </c>
       <c r="F19" s="0">
-        <v>0.41069417266666663</v>
+        <v>0.75913631856666663</v>
       </c>
       <c r="G19" s="0">
-        <v>0.62920039993333321</v>
+        <v>0.41467470911666671</v>
       </c>
       <c r="H19" s="0">
-        <v>0.40047356028333336</v>
+        <v>0.44171996159999993</v>
       </c>
       <c r="I19" s="0">
-        <v>0.14571350412333331</v>
+        <v>0.39577816643500002</v>
       </c>
       <c r="J19" s="0">
-        <v>1.1252735353266665</v>
+        <v>0.49899983623333333</v>
       </c>
       <c r="K19" s="0">
-        <v>0.52439710351666668</v>
+        <v>0.11235793074333331</v>
       </c>
       <c r="L19" s="0">
-        <v>0.81578174930000003</v>
+        <v>0.60962695138166667</v>
       </c>
       <c r="M19" s="0">
-        <v>0.39577228165</v>
+        <v>0.37081020027999995</v>
       </c>
       <c r="N19" s="0">
-        <v>-0.27881399235000004</v>
+        <v>0.42421425010166669</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>0.33890814162499999</v>
+        <v>0.50277829390000006</v>
       </c>
       <c r="B20" s="0">
-        <v>0.22793797531666668</v>
+        <v>0.43094113459166666</v>
       </c>
       <c r="C20" s="0">
-        <v>-0.32569306587000008</v>
+        <v>0.28855692116500004</v>
       </c>
       <c r="D20" s="0">
-        <v>-0.17389023594166669</v>
+        <v>0.10610579861666672</v>
       </c>
       <c r="E20" s="0">
-        <v>-0.08060373013666669</v>
+        <v>0.26135314125000003</v>
       </c>
       <c r="F20" s="0">
-        <v>-0.571422973025</v>
+        <v>0.2962775021166667</v>
       </c>
       <c r="G20" s="0">
-        <v>-0.56759387847333331</v>
+        <v>0.21797397511666666</v>
       </c>
       <c r="H20" s="0">
-        <v>-0.013810909816666689</v>
+        <v>0.52288368845666666</v>
       </c>
       <c r="I20" s="0">
-        <v>0.01356608936500002</v>
+        <v>0.29583919099333333</v>
       </c>
       <c r="J20" s="0">
-        <v>0.31745401874999996</v>
+        <v>0.60173571744999999</v>
       </c>
       <c r="K20" s="0">
-        <v>-0.14499999763333332</v>
+        <v>0.38827155164999999</v>
       </c>
       <c r="L20" s="0">
-        <v>-0.090968284983333342</v>
+        <v>-0.63430318763333327</v>
       </c>
       <c r="M20" s="0">
-        <v>0.24881864154999994</v>
+        <v>-0.20421211315333332</v>
       </c>
       <c r="N20" s="0">
-        <v>-0.21565773274099997</v>
+        <v>-1.0708333430666668</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>-0.14372402052666666</v>
+        <v>-0.093196238319999999</v>
       </c>
       <c r="B21" s="0">
-        <v>0.062963431473333345</v>
+        <v>0.067642429756000003</v>
       </c>
       <c r="C21" s="0">
-        <v>0.072119454319999998</v>
+        <v>-0.26240672872000004</v>
       </c>
       <c r="D21" s="0">
-        <v>-0.23024074539999997</v>
+        <v>-0.81127373555999993</v>
       </c>
       <c r="E21" s="0">
-        <v>-0.49331701889999996</v>
+        <v>-0.5299357707333332</v>
       </c>
       <c r="F21" s="0">
-        <v>0.26565913257000001</v>
+        <v>-0.02509608977666665</v>
       </c>
       <c r="G21" s="0">
-        <v>0.32038705128466666</v>
+        <v>0.24721106582900002</v>
       </c>
       <c r="H21" s="0">
-        <v>-0.18917714687466664</v>
+        <v>0.54547089014799999</v>
       </c>
       <c r="I21" s="0">
-        <v>-0.083246613366666639</v>
+        <v>0.14020470941786667</v>
       </c>
       <c r="J21" s="0">
-        <v>-1.273379114495</v>
+        <v>0.25434605746999994</v>
       </c>
       <c r="K21" s="0">
-        <v>-0.63331396656666672</v>
+        <v>-0.46117669690333329</v>
       </c>
       <c r="L21" s="0">
-        <v>0.17109437843333331</v>
+        <v>-0.54760072456666664</v>
       </c>
       <c r="M21" s="0">
-        <v>-0.79911334313333338</v>
+        <v>-1.2936589711333333</v>
       </c>
       <c r="N21" s="0">
-        <v>0.021246020899999996</v>
+        <v>0.27931304216666669</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>-1.07671038575</v>
+        <v>-0.90064119534999998</v>
       </c>
       <c r="B22" s="0">
-        <v>-0.85940960614999995</v>
+        <v>-1.4880156264</v>
       </c>
       <c r="C22" s="0">
-        <v>-0.40870458414999999</v>
+        <v>-1.55508486195</v>
       </c>
       <c r="D22" s="0">
-        <v>-0.24469247882</v>
+        <v>-0.75387995780499995</v>
       </c>
       <c r="E22" s="0">
-        <v>0.18341457480000009</v>
+        <v>-0.59993654406499997</v>
       </c>
       <c r="F22" s="0">
-        <v>0.019802264189999946</v>
+        <v>-1.1633634339899999</v>
       </c>
       <c r="G22" s="0">
-        <v>-0.28951177683000001</v>
+        <v>-1.0833531037549999</v>
       </c>
       <c r="H22" s="0">
-        <v>0.048515267400000062</v>
+        <v>-0.79161177437999997</v>
       </c>
       <c r="I22" s="0">
-        <v>0.028171169150000064</v>
+        <v>-0.94881597811500007</v>
       </c>
       <c r="J22" s="0">
-        <v>0.22983989491000001</v>
+        <v>-0.91018465554999994</v>
       </c>
       <c r="K22" s="0">
-        <v>-1.23616272695</v>
+        <v>-2.4540861572499999</v>
       </c>
       <c r="L22" s="0">
-        <v>-0.35661244784999996</v>
+        <v>-1.4255627748499999</v>
       </c>
       <c r="M22" s="0">
-        <v>0.23700674534999999</v>
+        <v>-0.75756828504999985</v>
       </c>
       <c r="N22" s="0">
-        <v>-0.62363465549999997</v>
+        <v>-1.4963062539</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>0.3724697014433333</v>
+        <v>0.61443232928333336</v>
       </c>
       <c r="B23" s="0">
-        <v>0.72284668002999997</v>
+        <v>0.42205905501666674</v>
       </c>
       <c r="C23" s="0">
-        <v>0.82636568786666675</v>
+        <v>1.1868721015999999</v>
       </c>
       <c r="D23" s="0">
-        <v>-0.24787674645166666</v>
+        <v>0.7240049161933334</v>
       </c>
       <c r="E23" s="0">
-        <v>-0.10851196063333333</v>
+        <v>0.20827814885333334</v>
       </c>
       <c r="F23" s="0">
-        <v>0.54822908981666663</v>
+        <v>0.36950903363333332</v>
       </c>
       <c r="G23" s="0">
-        <v>0.81872228849666662</v>
+        <v>0.35125149596833327</v>
       </c>
       <c r="H23" s="0">
-        <v>0.46764084031666669</v>
+        <v>-0.07017757056666668</v>
       </c>
       <c r="I23" s="0">
-        <v>0.32912644728166662</v>
+        <v>0.923101647671</v>
       </c>
       <c r="J23" s="0">
-        <v>-0.31525827962333342</v>
+        <v>0.45609759153333318</v>
       </c>
       <c r="K23" s="0">
-        <v>1.0587648675999999</v>
+        <v>1.9754477746166668</v>
       </c>
       <c r="L23" s="0">
-        <v>-0.1398522173816667</v>
+        <v>-1.0628934495366666</v>
       </c>
       <c r="M23" s="0">
-        <v>-0.42029676055000004</v>
+        <v>0.076000482803333352</v>
       </c>
       <c r="N23" s="0">
-        <v>-1.0703921567333334</v>
+        <v>0.52058585691666659</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>-0.35143660153833334</v>
+        <v>-0.00092177035000000351</v>
       </c>
       <c r="B24" s="0">
-        <v>0.13676906439666664</v>
+        <v>0.022293640633333334</v>
       </c>
       <c r="C24" s="0">
-        <v>-0.052293212700000022</v>
+        <v>0.32608140825333337</v>
       </c>
       <c r="D24" s="0">
-        <v>-0.38694697412666668</v>
+        <v>-0.55155432980000008</v>
       </c>
       <c r="E24" s="0">
-        <v>-0.41738008129633331</v>
+        <v>-0.80949837079166653</v>
       </c>
       <c r="F24" s="0">
-        <v>-0.024090379119999998</v>
+        <v>0.14978607399166669</v>
       </c>
       <c r="G24" s="0">
-        <v>0.063090019388333321</v>
+        <v>0.26437230797333333</v>
       </c>
       <c r="H24" s="0">
-        <v>-0.21296685790666667</v>
+        <v>-0.23131013349999996</v>
       </c>
       <c r="I24" s="0">
-        <v>-0.17179625858333333</v>
+        <v>-0.12871660772333338</v>
       </c>
       <c r="J24" s="0">
-        <v>-0.077348201773333319</v>
+        <v>0.012355252900666663</v>
       </c>
       <c r="K24" s="0">
-        <v>0.1221041213166667</v>
+        <v>0.53342980523333328</v>
       </c>
       <c r="L24" s="0">
-        <v>0.37610306753433331</v>
+        <v>1.1294343261666668</v>
       </c>
       <c r="M24" s="0">
-        <v>-0.72730801048333338</v>
+        <v>-0.52238357093666665</v>
       </c>
       <c r="N24" s="0">
-        <v>-0.25597110142333324</v>
+        <v>0.51478668578333342</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>-0.85332599200000003</v>
+        <v>0.73007993276500005</v>
       </c>
       <c r="B25" s="0">
-        <v>-0.28670905555499998</v>
+        <v>0.64663559684999994</v>
       </c>
       <c r="C25" s="0">
-        <v>-0.60950475684999994</v>
+        <v>-0.22087175004999998</v>
       </c>
       <c r="D25" s="0">
-        <v>0.6653875159</v>
+        <v>-0.28986285065000006</v>
       </c>
       <c r="E25" s="0">
-        <v>-0.53102219010499996</v>
+        <v>-0.61201334190000001</v>
       </c>
       <c r="F25" s="0">
-        <v>-1.5034220675999999</v>
+        <v>-0.024146965700000023</v>
       </c>
       <c r="G25" s="0">
-        <v>-0.72119029980000005</v>
+        <v>0.18022088344999998</v>
       </c>
       <c r="H25" s="0">
-        <v>-0.82068951010000002</v>
+        <v>-0.335391094</v>
       </c>
       <c r="I25" s="0">
-        <v>-1.009957485245</v>
+        <v>-0.40228371213499997</v>
       </c>
       <c r="J25" s="0">
-        <v>-1.2321475448500001</v>
+        <v>-0.80264156341999993</v>
       </c>
       <c r="K25" s="0">
-        <v>-0.66651780257499993</v>
+        <v>0.26054610545000001</v>
       </c>
       <c r="L25" s="0">
-        <v>-0.26020521244999995</v>
+        <v>1.1547407105850001</v>
       </c>
       <c r="M25" s="0">
-        <v>-1.29321823655</v>
+        <v>-0.78609580042800009</v>
       </c>
       <c r="N25" s="0">
-        <v>0.44395407114999996</v>
+        <v>1.1268112194</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>0.32358827893666664</v>
+        <v>0.67201233888333334</v>
       </c>
       <c r="B26" s="0">
-        <v>0.70381192316666663</v>
+        <v>0.83562987995333327</v>
       </c>
       <c r="C26" s="0">
-        <v>0.08255968666666666</v>
+        <v>0.24538996025999998</v>
       </c>
       <c r="D26" s="0">
-        <v>-0.62593282419999996</v>
+        <v>0.13369439796666668</v>
       </c>
       <c r="E26" s="0">
-        <v>-0.77322602569999999</v>
+        <v>0.066256438155000041</v>
       </c>
       <c r="F26" s="0">
-        <v>-0.0096531923433333389</v>
+        <v>0.067916792251666663</v>
       </c>
       <c r="G26" s="0">
-        <v>-0.25461113325000001</v>
+        <v>-0.083791405253333312</v>
       </c>
       <c r="H26" s="0">
-        <v>0.12861845423333335</v>
+        <v>0.15140671145000004</v>
       </c>
       <c r="I26" s="0">
-        <v>0.65241948776666669</v>
+        <v>0.6070988584646666</v>
       </c>
       <c r="J26" s="0">
-        <v>0.35871545952999995</v>
+        <v>1.0476950934833333</v>
       </c>
       <c r="K26" s="0">
-        <v>-0.14591825131266667</v>
+        <v>0.51051568606666664</v>
       </c>
       <c r="L26" s="0">
-        <v>0.061507917733333348</v>
+        <v>1.0387171664833335</v>
       </c>
       <c r="M26" s="0">
-        <v>-1.2199266814</v>
+        <v>-0.32182221625000001</v>
       </c>
       <c r="N26" s="0">
-        <v>0.7911496512666667</v>
+        <v>0.26017815001666666</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>-0.60596712483533333</v>
+        <v>-0.37542473376666663</v>
       </c>
       <c r="B27" s="0">
-        <v>-0.59703617449333324</v>
+        <v>-0.27649043035000004</v>
       </c>
       <c r="C27" s="0">
-        <v>-0.38043801174333336</v>
+        <v>0.21006463347033341</v>
       </c>
       <c r="D27" s="0">
-        <v>-0.64118195649999987</v>
+        <v>0.24902627810666664</v>
       </c>
       <c r="E27" s="0">
-        <v>-0.62675835894999987</v>
+        <v>0.31776254231833334</v>
       </c>
       <c r="F27" s="0">
-        <v>-0.25243275804399995</v>
+        <v>0.53825623682833323</v>
       </c>
       <c r="G27" s="0">
-        <v>-0.42957517082333335</v>
+        <v>-0.088752993366666755</v>
       </c>
       <c r="H27" s="0">
-        <v>-0.47138422516333334</v>
+        <v>-0.10552193402</v>
       </c>
       <c r="I27" s="0">
-        <v>-0.27276598703999999</v>
+        <v>0.016667520419999991</v>
       </c>
       <c r="J27" s="0">
-        <v>0.11563029368000005</v>
+        <v>0.84829624539999993</v>
       </c>
       <c r="K27" s="0">
-        <v>-1.3174835411000001</v>
+        <v>-0.20851153658333335</v>
       </c>
       <c r="L27" s="0">
-        <v>-1.2099525599983334</v>
+        <v>0.10182743605000005</v>
       </c>
       <c r="M27" s="0">
-        <v>-0.78765612625000003</v>
+        <v>-0.13616120108333335</v>
       </c>
       <c r="N27" s="0">
-        <v>-0.12113695971666671</v>
+        <v>0.58095045156666658</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>0.70533838076666666</v>
+        <v>0.23610620919666675</v>
       </c>
       <c r="B28" s="0">
-        <v>0.95205122513999996</v>
+        <v>0.78270366739999997</v>
       </c>
       <c r="C28" s="0">
-        <v>0.00085982578333332338</v>
+        <v>0.16800982930000008</v>
       </c>
       <c r="D28" s="0">
-        <v>-0.67935110903666673</v>
+        <v>-0.88571622726666666</v>
       </c>
       <c r="E28" s="0">
-        <v>-0.40043435140666672</v>
+        <v>-0.24646541114999998</v>
       </c>
       <c r="F28" s="0">
-        <v>-0.26954819915</v>
+        <v>0.32794158709999999</v>
       </c>
       <c r="G28" s="0">
-        <v>0.23957803293666668</v>
+        <v>0.72670456626666646</v>
       </c>
       <c r="H28" s="0">
-        <v>0.33000852651666668</v>
+        <v>0.27428327660000018</v>
       </c>
       <c r="I28" s="0">
-        <v>0.19282895692999999</v>
+        <v>0.36242718845000005</v>
       </c>
       <c r="J28" s="0">
-        <v>1.0425116668166665</v>
+        <v>0.63162079766666668</v>
       </c>
       <c r="K28" s="0">
-        <v>-0.25028331291333333</v>
+        <v>-0.083269858261666663</v>
       </c>
       <c r="L28" s="0">
-        <v>-0.06281376968333334</v>
+        <v>-0.18408701159999996</v>
       </c>
       <c r="M28" s="0">
-        <v>0.14238079235000001</v>
+        <v>-0.95057153425000007</v>
       </c>
       <c r="N28" s="0">
-        <v>0.41625455121666671</v>
+        <v>-0.1841922179333334</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>-0.067902887700000025</v>
+        <v>-0.38891414345333336</v>
       </c>
       <c r="B29" s="0">
-        <v>-0.366321768085</v>
+        <v>-0.39203542625000004</v>
       </c>
       <c r="C29" s="0">
-        <v>-0.10125255309666667</v>
+        <v>-0.16072830198333332</v>
       </c>
       <c r="D29" s="0">
-        <v>-0.16626454911933333</v>
+        <v>-0.1788832418066667</v>
       </c>
       <c r="E29" s="0">
-        <v>-0.34640219494999996</v>
+        <v>-0.43064302357333334</v>
       </c>
       <c r="F29" s="0">
-        <v>-0.40688227619666661</v>
+        <v>-0.43512676930499999</v>
       </c>
       <c r="G29" s="0">
-        <v>-0.2719532241</v>
+        <v>-0.50295225735000004</v>
       </c>
       <c r="H29" s="0">
-        <v>-0.52604671397900005</v>
+        <v>-0.56249337516333331</v>
       </c>
       <c r="I29" s="0">
-        <v>-0.31455218261666662</v>
+        <v>0.043096120930000009</v>
       </c>
       <c r="J29" s="0">
-        <v>-0.1191691335</v>
+        <v>-0.085037765725333309</v>
       </c>
       <c r="K29" s="0">
-        <v>-0.54188800036000007</v>
+        <v>-0.19735832144999998</v>
       </c>
       <c r="L29" s="0">
-        <v>-0.86536017786666664</v>
+        <v>-0.45348901661666674</v>
       </c>
       <c r="M29" s="0">
-        <v>-0.86789395268333336</v>
+        <v>-0.93939954596333342</v>
       </c>
       <c r="N29" s="0">
-        <v>-1.3579883951999998</v>
+        <v>-0.1863366806</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>-0.46742455310333331</v>
+        <v>-0.71729716489999995</v>
       </c>
       <c r="B30" s="0">
-        <v>-0.069712546769999995</v>
+        <v>0.040239599106666649</v>
       </c>
       <c r="C30" s="0">
-        <v>-0.42478019818333335</v>
+        <v>-0.20125056296666666</v>
       </c>
       <c r="D30" s="0">
-        <v>-0.41294646185000006</v>
+        <v>-0.37154751098666666</v>
       </c>
       <c r="E30" s="0">
-        <v>-0.89810138402333328</v>
+        <v>-0.88234208956666671</v>
       </c>
       <c r="F30" s="0">
-        <v>-0.82260340983666658</v>
+        <v>-0.56116787911866661</v>
       </c>
       <c r="G30" s="0">
-        <v>-0.71241868347333326</v>
+        <v>-0.4987375906</v>
       </c>
       <c r="H30" s="0">
-        <v>-1.1196862982666667</v>
+        <v>-1.0229037313606666</v>
       </c>
       <c r="I30" s="0">
-        <v>-0.7016269213166666</v>
+        <v>-0.74267572487666667</v>
       </c>
       <c r="J30" s="0">
-        <v>-1.0039566221833334</v>
+        <v>-1.1221694079833333</v>
       </c>
       <c r="K30" s="0">
-        <v>-0.71382538324999989</v>
+        <v>-0.71921152574333336</v>
       </c>
       <c r="L30" s="0">
-        <v>0.69419180766666666</v>
+        <v>0.26256218011666665</v>
       </c>
       <c r="M30" s="0">
-        <v>0.87224826026333335</v>
+        <v>-0.45516304735000002</v>
       </c>
       <c r="N30" s="0">
-        <v>0.43050485754666667</v>
+        <v>0.90843092708333328</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>0.44769649461</v>
+        <v>0.28437604851666665</v>
       </c>
       <c r="B31" s="0">
-        <v>0.328116556665</v>
+        <v>0.40927641950833332</v>
       </c>
       <c r="C31" s="0">
-        <v>-0.37449345671333334</v>
+        <v>0.057006657807333383</v>
       </c>
       <c r="D31" s="0">
-        <v>0.22918077503333337</v>
+        <v>0.15551563217933334</v>
       </c>
       <c r="E31" s="0">
-        <v>0.07597872142000002</v>
+        <v>0.12909777719999999</v>
       </c>
       <c r="F31" s="0">
-        <v>-0.065575041483333332</v>
+        <v>-0.41823312030549997</v>
       </c>
       <c r="G31" s="0">
-        <v>-0.18583546544999999</v>
+        <v>-0.083914549599999999</v>
       </c>
       <c r="H31" s="0">
-        <v>0.064537418040000016</v>
+        <v>0.071334133450000003</v>
       </c>
       <c r="I31" s="0">
-        <v>0.42854183876333329</v>
+        <v>0.16522850005166667</v>
       </c>
       <c r="J31" s="0">
-        <v>-0.30775712394999999</v>
+        <v>-0.60672229365200003</v>
       </c>
       <c r="K31" s="0">
-        <v>-0.65937898565666664</v>
+        <v>0.023436220331666646</v>
       </c>
       <c r="L31" s="0">
-        <v>-0.016594208189999904</v>
+        <v>0.16630258545333332</v>
       </c>
       <c r="M31" s="0">
-        <v>0.63146997771666658</v>
+        <v>-0.0086825651396667258</v>
       </c>
       <c r="N31" s="0">
-        <v>-0.20471467841999991</v>
+        <v>-0.58184341248333338</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>0.40201351323866669</v>
+        <v>0.41432273774999995</v>
       </c>
       <c r="B32" s="0">
-        <v>0.73143990927333336</v>
+        <v>0.56719136253500002</v>
       </c>
       <c r="C32" s="0">
-        <v>0.81431188217166672</v>
+        <v>0.84192786111666673</v>
       </c>
       <c r="D32" s="0">
-        <v>0.59535092407000001</v>
+        <v>0.32478037835833334</v>
       </c>
       <c r="E32" s="0">
-        <v>0.40985154323</v>
+        <v>0.57582237076656662</v>
       </c>
       <c r="F32" s="0">
-        <v>0.33635196471333334</v>
+        <v>0.33294900445666664</v>
       </c>
       <c r="G32" s="0">
-        <v>0.14257844895333333</v>
+        <v>0.56985658331516664</v>
       </c>
       <c r="H32" s="0">
-        <v>-0.094080407285999992</v>
+        <v>0.35059113461066671</v>
       </c>
       <c r="I32" s="0">
-        <v>1.0258729931500001</v>
+        <v>0.57151820531666664</v>
       </c>
       <c r="J32" s="0">
-        <v>0.95505138110666676</v>
+        <v>0.30350562506666667</v>
       </c>
       <c r="K32" s="0">
-        <v>0.40406620483</v>
+        <v>0.61694751801666659</v>
       </c>
       <c r="L32" s="0">
-        <v>0.35325586157666666</v>
+        <v>0.023511466016666704</v>
       </c>
       <c r="M32" s="0">
-        <v>0.3098250229666667</v>
+        <v>0.36251789795</v>
       </c>
       <c r="N32" s="0">
-        <v>1.9128608842333332</v>
+        <v>0.25991324537833332</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>-0.10009331824333334</v>
+        <v>-0.19688969036666668</v>
       </c>
       <c r="B33" s="0">
-        <v>-0.090814535400000007</v>
+        <v>0.28852081546666669</v>
       </c>
       <c r="C33" s="0">
-        <v>-1.1201063555333335</v>
+        <v>0.42745334966666665</v>
       </c>
       <c r="D33" s="0">
-        <v>-0.61021989472299998</v>
+        <v>-0.032631471683000013</v>
       </c>
       <c r="E33" s="0">
-        <v>-0.43121769427333334</v>
+        <v>-0.15717551820666667</v>
       </c>
       <c r="F33" s="0">
-        <v>-0.70626923024333343</v>
+        <v>0.13689384605933336</v>
       </c>
       <c r="G33" s="0">
-        <v>-0.20327011836</v>
+        <v>0.35284896070999999</v>
       </c>
       <c r="H33" s="0">
-        <v>0.31913990999666669</v>
+        <v>0.33171607587000002</v>
       </c>
       <c r="I33" s="0">
-        <v>-0.70379131509999993</v>
+        <v>0.025393328443333342</v>
       </c>
       <c r="J33" s="0">
-        <v>-0.66136415355333344</v>
+        <v>-0.47644899270333324</v>
       </c>
       <c r="K33" s="0">
-        <v>0.19671776373333338</v>
+        <v>0.65108875412666667</v>
       </c>
       <c r="L33" s="0">
-        <v>-0.95300694173333333</v>
+        <v>-0.45256817156666662</v>
       </c>
       <c r="M33" s="0">
-        <v>-0.42569964152333334</v>
+        <v>-0.47453313067666664</v>
       </c>
       <c r="N33" s="0">
-        <v>-0.87595323731333319</v>
+        <v>-0.34579710056666668</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>0.80392420706666667</v>
+        <v>0.082158370466666658</v>
       </c>
       <c r="B34" s="0">
-        <v>0.57513760827999993</v>
+        <v>0.095401130943333384</v>
       </c>
       <c r="C34" s="0">
-        <v>0.16927851818833334</v>
+        <v>0.10878771819333333</v>
       </c>
       <c r="D34" s="0">
-        <v>0.43455195332666663</v>
+        <v>-0.067272276196666661</v>
       </c>
       <c r="E34" s="0">
-        <v>0.70735021459666669</v>
+        <v>0.13051313172999998</v>
       </c>
       <c r="F34" s="0">
-        <v>0.44764471701666664</v>
+        <v>-0.090973817286666675</v>
       </c>
       <c r="G34" s="0">
-        <v>0.46464642624200003</v>
+        <v>0.23862365577833333</v>
       </c>
       <c r="H34" s="0">
-        <v>0.25119426845949999</v>
+        <v>-0.103013395965</v>
       </c>
       <c r="I34" s="0">
-        <v>0.59119783935833325</v>
+        <v>0.26109358264166665</v>
       </c>
       <c r="J34" s="0">
-        <v>-0.2117017600633333</v>
+        <v>-0.32604026978333334</v>
       </c>
       <c r="K34" s="0">
-        <v>0.25765104475666667</v>
+        <v>0.20631187445633337</v>
       </c>
       <c r="L34" s="0">
-        <v>-0.06011096769999999</v>
+        <v>0.16844953996166667</v>
       </c>
       <c r="M34" s="0">
-        <v>-0.28670454514999999</v>
+        <v>-0.74643451478</v>
       </c>
       <c r="N34" s="0">
-        <v>0.44914640090000002</v>
+        <v>-0.31621671029666654</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>-0.74170081826666667</v>
+        <v>-0.5942146287086667</v>
       </c>
       <c r="B35" s="0">
-        <v>-0.70445419003333332</v>
+        <v>-0.58895816398333334</v>
       </c>
       <c r="C35" s="0">
-        <v>-0.40330263294333335</v>
+        <v>-0.84858496292499996</v>
       </c>
       <c r="D35" s="0">
-        <v>-0.39423666399666668</v>
+        <v>-0.81324966121666664</v>
       </c>
       <c r="E35" s="0">
-        <v>-0.27327127874666657</v>
+        <v>-0.53059931952333328</v>
       </c>
       <c r="F35" s="0">
-        <v>-0.76789341109499998</v>
+        <v>-0.55229838515000007</v>
       </c>
       <c r="G35" s="0">
-        <v>-0.26913667556666671</v>
+        <v>0.38395981049666666</v>
       </c>
       <c r="H35" s="0">
-        <v>-0.39272683597000002</v>
+        <v>0.14191971037523332</v>
       </c>
       <c r="I35" s="0">
-        <v>-0.29238036984333338</v>
+        <v>-0.59530710127166664</v>
       </c>
       <c r="J35" s="0">
-        <v>0.13004406438333335</v>
+        <v>-0.86229596600000002</v>
       </c>
       <c r="K35" s="0">
-        <v>-0.60857877357166679</v>
+        <v>-0.73877230590333332</v>
       </c>
       <c r="L35" s="0">
-        <v>-0.1905210437116667</v>
+        <v>0.043951333706666665</v>
       </c>
       <c r="M35" s="0">
-        <v>0.022137245216666671</v>
+        <v>0.017304447724000027</v>
       </c>
       <c r="N35" s="0">
-        <v>-0.92638429508333331</v>
+        <v>-1.7495569680666667</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>-0.092627266563333338</v>
+        <v>0.24448892750666668</v>
       </c>
       <c r="B36" s="0">
-        <v>-0.81462348293333331</v>
+        <v>-0.1685615590666667</v>
       </c>
       <c r="C36" s="0">
-        <v>-0.83368576761666668</v>
+        <v>-0.17511233072333332</v>
       </c>
       <c r="D36" s="0">
-        <v>-0.34370840135833336</v>
+        <v>-0.10525112477666668</v>
       </c>
       <c r="E36" s="0">
-        <v>-0.29797596065666665</v>
+        <v>-0.193989782985</v>
       </c>
       <c r="F36" s="0">
-        <v>-0.48891240423999999</v>
+        <v>-0.14399281758983334</v>
       </c>
       <c r="G36" s="0">
-        <v>-1.1254021461833332</v>
+        <v>-0.45860231955333336</v>
       </c>
       <c r="H36" s="0">
-        <v>-0.49772941211999999</v>
+        <v>-0.42622252651333331</v>
       </c>
       <c r="I36" s="0">
-        <v>0.0014573580266667163</v>
+        <v>-0.13689266396999997</v>
       </c>
       <c r="J36" s="0">
-        <v>0.94837410718333337</v>
+        <v>0.5678823109133333</v>
       </c>
       <c r="K36" s="0">
-        <v>-0.25020511909999998</v>
+        <v>-0.39607440858333332</v>
       </c>
       <c r="L36" s="0">
-        <v>0.68366668136666675</v>
+        <v>1.3372916350399999</v>
       </c>
       <c r="M36" s="0">
-        <v>-0.11367931433000002</v>
+        <v>1.0942135007333333</v>
       </c>
       <c r="N36" s="0">
-        <v>1.842002904279</v>
+        <v>2.1058353921491664</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>0.23311992267599996</v>
+        <v>0.027731572783333325</v>
       </c>
       <c r="B37" s="0">
-        <v>0.72253171155000007</v>
+        <v>-0.157296365065</v>
       </c>
       <c r="C37" s="0">
-        <v>0.59745791054333341</v>
+        <v>-0.49299605755333331</v>
       </c>
       <c r="D37" s="0">
-        <v>-0.094510728533333366</v>
+        <v>0.25519922733333333</v>
       </c>
       <c r="E37" s="0">
-        <v>-0.4813107334333333</v>
+        <v>0.63227893107333333</v>
       </c>
       <c r="F37" s="0">
-        <v>0.49599987420000002</v>
+        <v>-0.26337898168333335</v>
       </c>
       <c r="G37" s="0">
-        <v>1.1703568898333334</v>
+        <v>-0.012552094999999985</v>
       </c>
       <c r="H37" s="0">
-        <v>0.56130283908666656</v>
+        <v>0.29303223950000001</v>
       </c>
       <c r="I37" s="0">
-        <v>-0.41115916531666674</v>
+        <v>0.16228069521666666</v>
       </c>
       <c r="J37" s="0">
-        <v>1.2830166032333332</v>
+        <v>0.044724593363333322</v>
       </c>
       <c r="K37" s="0">
-        <v>0.67760566701666658</v>
+        <v>-0.38583033574999998</v>
       </c>
       <c r="L37" s="0">
-        <v>0.71922522656666654</v>
+        <v>-0.30534163196333336</v>
       </c>
       <c r="M37" s="0">
-        <v>0.27586807111999978</v>
+        <v>0.24890272941666666</v>
       </c>
       <c r="N37" s="0">
-        <v>0.05568280238333323</v>
+        <v>-0.66852646771000002</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>0.031852856746666672</v>
+        <v>0.015604127249999988</v>
       </c>
       <c r="B38" s="0">
-        <v>0.15305605318333332</v>
+        <v>-0.12346830152666666</v>
       </c>
       <c r="C38" s="0">
-        <v>0.43221505085</v>
+        <v>-0.27758865391000004</v>
       </c>
       <c r="D38" s="0">
-        <v>0.61483083606999989</v>
+        <v>0.29979493971666665</v>
       </c>
       <c r="E38" s="0">
-        <v>0.59783654696999999</v>
+        <v>0.52161280440000013</v>
       </c>
       <c r="F38" s="0">
-        <v>0.57113807828333341</v>
+        <v>0.11265009943333337</v>
       </c>
       <c r="G38" s="0">
-        <v>0.75114059594999993</v>
+        <v>-0.15293394968333335</v>
       </c>
       <c r="H38" s="0">
-        <v>0.54034580328000004</v>
+        <v>0.32043445427333339</v>
       </c>
       <c r="I38" s="0">
-        <v>0.20020081953333332</v>
+        <v>0.84678775468</v>
       </c>
       <c r="J38" s="0">
-        <v>1.0810597551333334</v>
+        <v>0.8996645376950001</v>
       </c>
       <c r="K38" s="0">
-        <v>0.19093991506666666</v>
+        <v>-0.25821544006666675</v>
       </c>
       <c r="L38" s="0">
-        <v>-0.6088287706033334</v>
+        <v>-0.08140479673833334</v>
       </c>
       <c r="M38" s="0">
-        <v>0.040181050750000009</v>
+        <v>0.10332911816666671</v>
       </c>
       <c r="N38" s="0">
-        <v>-0.66170248498333328</v>
+        <v>1.1096054210166666</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>0.65332171404333328</v>
+        <v>-0.23273074489666667</v>
       </c>
       <c r="B39" s="0">
-        <v>0.77776544141666659</v>
+        <v>0.092362866210000061</v>
       </c>
       <c r="C39" s="0">
-        <v>1.0882695543566665</v>
+        <v>0.1254224084783333</v>
       </c>
       <c r="D39" s="0">
-        <v>0.50697592057000007</v>
+        <v>-0.30596073621666658</v>
       </c>
       <c r="E39" s="0">
-        <v>0.18764408974666669</v>
+        <v>-0.20071782328333335</v>
       </c>
       <c r="F39" s="0">
-        <v>0.71741824985826663</v>
+        <v>0.61091496624999997</v>
       </c>
       <c r="G39" s="0">
-        <v>1.0504950648666667</v>
+        <v>0.97807757883333324</v>
       </c>
       <c r="H39" s="0">
-        <v>0.55044439506666665</v>
+        <v>0.55548284136666659</v>
       </c>
       <c r="I39" s="0">
-        <v>0.31067253317499999</v>
+        <v>-0.36402851396383329</v>
       </c>
       <c r="J39" s="0">
-        <v>0.48211463099999996</v>
+        <v>-0.15645285080000004</v>
       </c>
       <c r="K39" s="0">
-        <v>0.99735001290000003</v>
+        <v>0.12768882933333336</v>
       </c>
       <c r="L39" s="0">
-        <v>1.6925551128666669</v>
+        <v>0.14555513008333332</v>
       </c>
       <c r="M39" s="0">
-        <v>0.71481097260000004</v>
+        <v>0.8097712175166667</v>
       </c>
       <c r="N39" s="0">
-        <v>-0.014398186233333221</v>
+        <v>0.07644503665000002</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>-0.025295919909999992</v>
+        <v>0.39821608280000004</v>
       </c>
       <c r="B40" s="0">
-        <v>-0.43084732425000005</v>
+        <v>0.44340493209999998</v>
       </c>
       <c r="C40" s="0">
-        <v>-0.11100504673316658</v>
+        <v>0.62130715731666664</v>
       </c>
       <c r="D40" s="0">
-        <v>0.30880581090500003</v>
+        <v>0.097266166168333321</v>
       </c>
       <c r="E40" s="0">
-        <v>0.42810463027000001</v>
+        <v>0.27155624615000001</v>
       </c>
       <c r="F40" s="0">
-        <v>0.94808861866666672</v>
+        <v>0.42110336300666662</v>
       </c>
       <c r="G40" s="0">
-        <v>0.59496298870566666</v>
+        <v>0.24131370521500001</v>
       </c>
       <c r="H40" s="0">
-        <v>0.15163416305000002</v>
+        <v>-0.13385034828666667</v>
       </c>
       <c r="I40" s="0">
-        <v>-0.016399855297666716</v>
+        <v>0.033476193362666669</v>
       </c>
       <c r="J40" s="0">
-        <v>-0.74598932181200006</v>
+        <v>0.15604445419833329</v>
       </c>
       <c r="K40" s="0">
-        <v>-0.62144611471666666</v>
+        <v>0.16556464798333334</v>
       </c>
       <c r="L40" s="0">
-        <v>-0.30491024444000003</v>
+        <v>-0.096610086690000055</v>
       </c>
       <c r="M40" s="0">
-        <v>0.080250697216666556</v>
+        <v>-0.65374184902333332</v>
       </c>
       <c r="N40" s="0">
-        <v>0.15908466166666668</v>
+        <v>0.81075226711000004</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>0.33407394438666665</v>
+        <v>-0.47044576831000001</v>
       </c>
       <c r="B41" s="0">
-        <v>0.45701324462999998</v>
+        <v>-0.49869973428333336</v>
       </c>
       <c r="C41" s="0">
-        <v>0.46532307951666668</v>
+        <v>-0.27452162996166674</v>
       </c>
       <c r="D41" s="0">
-        <v>0.3228359466166667</v>
+        <v>-0.29614888540333334</v>
       </c>
       <c r="E41" s="0">
-        <v>-0.47810911919333332</v>
+        <v>-0.92374328409999995</v>
       </c>
       <c r="F41" s="0">
-        <v>0.46347066283333338</v>
+        <v>0.37696433708333332</v>
       </c>
       <c r="G41" s="0">
-        <v>0.12194847480000004</v>
+        <v>-0.12550261453849998</v>
       </c>
       <c r="H41" s="0">
-        <v>0.44611883298333332</v>
+        <v>0.19045831271499994</v>
       </c>
       <c r="I41" s="0">
-        <v>0.10037993176333332</v>
+        <v>-0.46687037517999996</v>
       </c>
       <c r="J41" s="0">
-        <v>0.26357293152333328</v>
+        <v>0.0041823913216665898</v>
       </c>
       <c r="K41" s="0">
-        <v>0.97903844362999992</v>
+        <v>0.24089012290166673</v>
       </c>
       <c r="L41" s="0">
-        <v>0.66167742659666673</v>
+        <v>0.21567761105</v>
       </c>
       <c r="M41" s="0">
-        <v>0.1127633930999999</v>
+        <v>-0.57462168506</v>
       </c>
       <c r="N41" s="0">
-        <v>0.5889146513900001</v>
+        <v>0.44663763710000004</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>-0.46849835063333339</v>
+        <v>-0.52583207300000001</v>
       </c>
       <c r="B42" s="0">
-        <v>-0.084184864183333319</v>
+        <v>-0.0062225852150000205</v>
       </c>
       <c r="C42" s="0">
-        <v>0.011200228016666647</v>
+        <v>0.28182648213333333</v>
       </c>
       <c r="D42" s="0">
-        <v>-0.37584419966666671</v>
+        <v>-0.33161000530000001</v>
       </c>
       <c r="E42" s="0">
-        <v>-0.39889852823000005</v>
+        <v>-0.53327829430000007</v>
       </c>
       <c r="F42" s="0">
-        <v>0.55780980723333329</v>
+        <v>0.28238270441666669</v>
       </c>
       <c r="G42" s="0">
-        <v>1.0587046852333333</v>
+        <v>0.88949821270666662</v>
       </c>
       <c r="H42" s="0">
-        <v>0.73958490151</v>
+        <v>0.47769516665</v>
       </c>
       <c r="I42" s="0">
-        <v>-0.26138814621666667</v>
+        <v>-0.23009326515966666</v>
       </c>
       <c r="J42" s="0">
-        <v>0.94657542660333316</v>
+        <v>1.5797803772666668</v>
       </c>
       <c r="K42" s="0">
-        <v>-0.54648134543333338</v>
+        <v>-0.019549582666666704</v>
       </c>
       <c r="L42" s="0">
-        <v>-0.039188112016666762</v>
+        <v>0.23581473435</v>
       </c>
       <c r="M42" s="0">
-        <v>0.21783972900333332</v>
+        <v>0.22540612364999998</v>
       </c>
       <c r="N42" s="0">
-        <v>-0.89934144153166673</v>
+        <v>0.0099862516133333301</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>-0.016159897479999998</v>
+        <v>-0.19136842955166664</v>
       </c>
       <c r="B43" s="0">
-        <v>0.2417857233166667</v>
+        <v>-0.12724463672</v>
       </c>
       <c r="C43" s="0">
-        <v>0.62902315738333336</v>
+        <v>-0.0052018197583333647</v>
       </c>
       <c r="D43" s="0">
-        <v>0.5511902117466666</v>
+        <v>0.24416792739999998</v>
       </c>
       <c r="E43" s="0">
-        <v>0.43859044717999995</v>
+        <v>0.31665086703333334</v>
       </c>
       <c r="F43" s="0">
-        <v>1.57438371565</v>
+        <v>0.84525030493333331</v>
       </c>
       <c r="G43" s="0">
-        <v>0.90550348366666666</v>
+        <v>0.16296630865666656</v>
       </c>
       <c r="H43" s="0">
-        <v>0.62541361119999994</v>
+        <v>0.20964737637950001</v>
       </c>
       <c r="I43" s="0">
-        <v>-0.32151376476499999</v>
+        <v>-0.27526164223333338</v>
       </c>
       <c r="J43" s="0">
-        <v>0.6086664752833334</v>
+        <v>0.52353300691333327</v>
       </c>
       <c r="K43" s="0">
-        <v>0.79215420826666672</v>
+        <v>1.2364008034166667</v>
       </c>
       <c r="L43" s="0">
-        <v>0.28160190709999999</v>
+        <v>0.18214855785333331</v>
       </c>
       <c r="M43" s="0">
-        <v>0.092584886839500016</v>
+        <v>0.72516268016666663</v>
       </c>
       <c r="N43" s="0">
-        <v>-0.36689446496666667</v>
+        <v>-0.23969228176666668</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>0.61640003155</v>
+        <v>0.28949574089999996</v>
       </c>
       <c r="B44" s="0">
-        <v>0.36678262159000002</v>
+        <v>-0.054489323460000127</v>
       </c>
       <c r="C44" s="0">
-        <v>0.47719214378333324</v>
+        <v>0.36790246760000006</v>
       </c>
       <c r="D44" s="0">
-        <v>0.4036642207033333</v>
+        <v>0.082628650550000016</v>
       </c>
       <c r="E44" s="0">
-        <v>0.4330733882833333</v>
+        <v>0.59576440580000001</v>
       </c>
       <c r="F44" s="0">
-        <v>0.40625051355000003</v>
+        <v>0.21542645223666668</v>
       </c>
       <c r="G44" s="0">
-        <v>-0.035835752816666622</v>
+        <v>0.4006061207433334</v>
       </c>
       <c r="H44" s="0">
-        <v>0.60885315968333331</v>
+        <v>0.3936612460833333</v>
       </c>
       <c r="I44" s="0">
-        <v>0.56867985415</v>
+        <v>-0.10872614967666666</v>
       </c>
       <c r="J44" s="0">
-        <v>1.1353116459166666</v>
+        <v>1.1777275538999998</v>
       </c>
       <c r="K44" s="0">
-        <v>0.3361570080666666</v>
+        <v>0.64957801469999998</v>
       </c>
       <c r="L44" s="0">
-        <v>0.68989906388166655</v>
+        <v>-0.22698306960000003</v>
       </c>
       <c r="M44" s="0">
-        <v>0.55747232483333331</v>
+        <v>0.45790368860266673</v>
       </c>
       <c r="N44" s="0">
-        <v>1.3334622728999999</v>
+        <v>1.8411490580000001</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>-0.0026390317099999616</v>
+        <v>0.11669465929999989</v>
       </c>
       <c r="B45" s="0">
-        <v>-0.19970361439500003</v>
+        <v>-0.081573909744999951</v>
       </c>
       <c r="C45" s="0">
-        <v>-0.052809885000000015</v>
+        <v>0.084552081150000069</v>
       </c>
       <c r="D45" s="0">
-        <v>-0.5024259204</v>
+        <v>-0.10937413870000001</v>
       </c>
       <c r="E45" s="0">
-        <v>-0.70648730225</v>
+        <v>-0.47087883697499999</v>
       </c>
       <c r="F45" s="0">
-        <v>-0.12051273729499998</v>
+        <v>-0.27706861681499995</v>
       </c>
       <c r="G45" s="0">
-        <v>-0.43824320404999995</v>
+        <v>-0.66644861964999991</v>
       </c>
       <c r="H45" s="0">
-        <v>-0.45395721437000003</v>
+        <v>-0.59532432818499992</v>
       </c>
       <c r="I45" s="0">
-        <v>-0.52387495080000002</v>
+        <v>-0.48967194274999998</v>
       </c>
       <c r="J45" s="0">
-        <v>-0.27334905309999996</v>
+        <v>-0.04374407690000004</v>
       </c>
       <c r="K45" s="0">
-        <v>-0.21008501172999994</v>
+        <v>-0.3474051834250001</v>
       </c>
       <c r="L45" s="0">
-        <v>0.42568474265</v>
+        <v>0.38109273534999999</v>
       </c>
       <c r="M45" s="0">
-        <v>-0.026915761799999993</v>
+        <v>0.127473163</v>
       </c>
       <c r="N45" s="0">
-        <v>0.96998532814999994</v>
+        <v>1.0995783588500001</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>0.056492219250000003</v>
+        <v>0.51217405205333333</v>
       </c>
       <c r="B46" s="0">
-        <v>-0.59419792198666666</v>
+        <v>-0.45190164937333333</v>
       </c>
       <c r="C46" s="0">
-        <v>-1.10187679905</v>
+        <v>-0.86534873986666661</v>
       </c>
       <c r="D46" s="0">
-        <v>-0.71690869369999999</v>
+        <v>-0.66008002707333324</v>
       </c>
       <c r="E46" s="0">
-        <v>-0.13676045961666666</v>
+        <v>-0.37686788464999998</v>
       </c>
       <c r="F46" s="0">
-        <v>-0.52806946993999992</v>
+        <v>-0.50409887509333329</v>
       </c>
       <c r="G46" s="0">
-        <v>-0.361864482845</v>
+        <v>-0.36564209031666672</v>
       </c>
       <c r="H46" s="0">
-        <v>-0.20432332007499998</v>
+        <v>-0.20263201836233335</v>
       </c>
       <c r="I46" s="0">
-        <v>-1.0608584891166668</v>
+        <v>-0.78247841824999997</v>
       </c>
       <c r="J46" s="0">
-        <v>-1.3043535699399997</v>
+        <v>-1.8574312041999999</v>
       </c>
       <c r="K46" s="0">
-        <v>-1.1769363027333333</v>
+        <v>-1.1920906860666667</v>
       </c>
       <c r="L46" s="0">
-        <v>-1.0168346619833333</v>
+        <v>-0.77195516178333345</v>
       </c>
       <c r="M46" s="0">
-        <v>-1.1130521739666666</v>
+        <v>-1.2205709553499999</v>
       </c>
       <c r="N46" s="0">
-        <v>-1.4204859533</v>
+        <v>-0.6692067889333333</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>-0.00058272852500002026</v>
+        <v>-0.25796456528</v>
       </c>
       <c r="B47" s="0">
-        <v>0.31766505769000003</v>
+        <v>-0.10462050645500001</v>
       </c>
       <c r="C47" s="0">
-        <v>0.49704602931500008</v>
+        <v>0.017802199500000004</v>
       </c>
       <c r="D47" s="0">
-        <v>0.09156809669999999</v>
+        <v>-0.0043789061500000281</v>
       </c>
       <c r="E47" s="0">
-        <v>0.27570518815</v>
+        <v>-0.07848503754999997</v>
       </c>
       <c r="F47" s="0">
-        <v>0.55787468164999998</v>
+        <v>0.13923722230000002</v>
       </c>
       <c r="G47" s="0">
-        <v>0.71715214814999995</v>
+        <v>0.04602055464999999</v>
       </c>
       <c r="H47" s="0">
-        <v>0.28493785230000002</v>
+        <v>-0.086385999349999992</v>
       </c>
       <c r="I47" s="0">
-        <v>0.079265633849999961</v>
+        <v>0.097794148049999988</v>
       </c>
       <c r="J47" s="0">
-        <v>0.11896127255</v>
+        <v>0.30164967235000001</v>
       </c>
       <c r="K47" s="0">
-        <v>0.8924218852050001</v>
+        <v>0.84444941924000005</v>
       </c>
       <c r="L47" s="0">
-        <v>0.18245016669999997</v>
+        <v>0.12690561543250004</v>
       </c>
       <c r="M47" s="0">
-        <v>-0.16390207304999999</v>
+        <v>0.54332651784999997</v>
       </c>
       <c r="N47" s="0">
-        <v>1.390620257448</v>
+        <v>1.5883927073000002</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>0.25408168654999996</v>
+        <v>0.90000210843000006</v>
       </c>
       <c r="B48" s="0">
-        <v>0.57783142245500008</v>
+        <v>0.82845445902500003</v>
       </c>
       <c r="C48" s="0">
-        <v>0.88301906084049997</v>
+        <v>1.0542499477499998</v>
       </c>
       <c r="D48" s="0">
-        <v>0.47816178522000002</v>
+        <v>0.61022365835000003</v>
       </c>
       <c r="E48" s="0">
-        <v>0.13667306149999997</v>
+        <v>0.29097717181999999</v>
       </c>
       <c r="F48" s="0">
-        <v>0.16108504395500001</v>
+        <v>0.42797787998500003</v>
       </c>
       <c r="G48" s="0">
-        <v>0.18126896284999999</v>
+        <v>0.26596995560500003</v>
       </c>
       <c r="H48" s="0">
-        <v>0.10789303024000001</v>
+        <v>0.34417060589999998</v>
       </c>
       <c r="I48" s="0">
-        <v>0.35563081459999996</v>
+        <v>0.34867526207999999</v>
       </c>
       <c r="J48" s="0">
-        <v>1.5247015525949998</v>
+        <v>0.9930054204955</v>
       </c>
       <c r="K48" s="0">
-        <v>-0.071715441072999986</v>
+        <v>0.79138140039999993</v>
       </c>
       <c r="L48" s="0">
-        <v>0.40522556750000005</v>
+        <v>0.47895617120000011</v>
       </c>
       <c r="M48" s="0">
-        <v>0.58991220359999996</v>
+        <v>0.75814560699999989</v>
       </c>
       <c r="N48" s="0">
-        <v>0.88360436459500002</v>
+        <v>1.3662520844500001</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>0.10800111406666668</v>
+        <v>0.56831165875</v>
       </c>
       <c r="B49" s="0">
-        <v>0.099259616735000028</v>
+        <v>0.33517936447000002</v>
       </c>
       <c r="C49" s="0">
-        <v>-0.16017284863333331</v>
+        <v>0.16373388035000003</v>
       </c>
       <c r="D49" s="0">
-        <v>-0.29127597768333335</v>
+        <v>0.11965944994999998</v>
       </c>
       <c r="E49" s="0">
-        <v>-0.27457033084333332</v>
+        <v>-0.085003828684999949</v>
       </c>
       <c r="F49" s="0">
-        <v>0.65742126763833331</v>
+        <v>0.37461137634999997</v>
       </c>
       <c r="G49" s="0">
-        <v>0.51799116985833327</v>
+        <v>0.84795990515000008</v>
       </c>
       <c r="H49" s="0">
-        <v>0.33191562148000003</v>
+        <v>0.64618651304999997</v>
       </c>
       <c r="I49" s="0">
-        <v>0.38073386837333328</v>
+        <v>0.24034622525000005</v>
       </c>
       <c r="J49" s="0">
-        <v>0.67936150574999998</v>
+        <v>0.51621820523499995</v>
       </c>
       <c r="K49" s="0">
-        <v>0.11301974092966667</v>
+        <v>-0.50958490899999997</v>
       </c>
       <c r="L49" s="0">
-        <v>0.87486726256666669</v>
+        <v>-0.40931051128000001</v>
       </c>
       <c r="M49" s="0">
-        <v>0.34132286492999997</v>
+        <v>0.19186221539499998</v>
       </c>
       <c r="N49" s="0">
-        <v>0.099007801499999978</v>
+        <v>-1.1051632372</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>1.1328043652799999</v>
+        <v>-0.033948460650000012</v>
       </c>
       <c r="B50" s="0">
-        <v>0.58113236369999999</v>
+        <v>-0.42256538571299984</v>
       </c>
       <c r="C50" s="0">
-        <v>0.30737056424999992</v>
+        <v>-0.92113025595000009</v>
       </c>
       <c r="D50" s="0">
-        <v>0.67400008249999999</v>
+        <v>-0.57540328201500002</v>
       </c>
       <c r="E50" s="0">
-        <v>0.22601570425</v>
+        <v>-1.2934449734</v>
       </c>
       <c r="F50" s="0">
-        <v>0.18139075980000002</v>
+        <v>-0.41243627423499996</v>
       </c>
       <c r="G50" s="0">
-        <v>0.82367077086999985</v>
+        <v>0.20928471844999974</v>
       </c>
       <c r="H50" s="0">
-        <v>0.85934649658999995</v>
+        <v>-0.017211599949999989</v>
       </c>
       <c r="I50" s="0">
-        <v>0.67649971648850005</v>
+        <v>-0.03178343035000003</v>
       </c>
       <c r="J50" s="0">
-        <v>1.8368234402949999</v>
+        <v>1.4239565588999998</v>
       </c>
       <c r="K50" s="0">
-        <v>1.0532507124500001</v>
+        <v>-0.49630176322500008</v>
       </c>
       <c r="L50" s="0">
-        <v>1.1342666863000002</v>
+        <v>-0.66025966889999987</v>
       </c>
       <c r="M50" s="0">
-        <v>0.36923891870000003</v>
+        <v>-1.0934824093</v>
       </c>
       <c r="N50" s="0">
-        <v>0.71734370889999988</v>
+        <v>-1.2465577702499999</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>0.23592819354999994</v>
+        <v>-0.57028617085000011</v>
       </c>
       <c r="B51" s="0">
-        <v>0.52860336649999995</v>
+        <v>-0.54767833494999996</v>
       </c>
       <c r="C51" s="0">
-        <v>1.0018505091199998</v>
+        <v>0.40312841209999994</v>
       </c>
       <c r="D51" s="0">
-        <v>0.93122125074999995</v>
+        <v>0.64520540550000005</v>
       </c>
       <c r="E51" s="0">
-        <v>0.89484876719500006</v>
+        <v>0.84695704689999995</v>
       </c>
       <c r="F51" s="0">
-        <v>0.55247141855000004</v>
+        <v>0.63426816375000006</v>
       </c>
       <c r="G51" s="0">
-        <v>0.80619174425000006</v>
+        <v>0.21107459378499993</v>
       </c>
       <c r="H51" s="0">
-        <v>0.49674432998499995</v>
+        <v>0.42299399913500002</v>
       </c>
       <c r="I51" s="0">
-        <v>0.52962672194999993</v>
+        <v>0.29373173081000004</v>
       </c>
       <c r="J51" s="0">
-        <v>0.41103107367000002</v>
+        <v>0.19072958120000005</v>
       </c>
       <c r="K51" s="0">
-        <v>0.957441283315</v>
+        <v>0.031060001849999984</v>
       </c>
       <c r="L51" s="0">
-        <v>1.4793591530000001</v>
+        <v>0.89281950579500002</v>
       </c>
       <c r="M51" s="0">
-        <v>1.40619936543</v>
+        <v>0.4358516281</v>
       </c>
       <c r="N51" s="0">
-        <v>1.8874680768500001</v>
+        <v>1.63443926585</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>-0.60043940160000009</v>
+        <v>-0.64041765225000002</v>
       </c>
       <c r="B52" s="0">
-        <v>-0.165540792035</v>
+        <v>0.099138715199999991</v>
       </c>
       <c r="C52" s="0">
-        <v>0.082731531684999998</v>
+        <v>0.061152871199999986</v>
       </c>
       <c r="D52" s="0">
-        <v>0.010376730350000085</v>
+        <v>-0.40271523245000002</v>
       </c>
       <c r="E52" s="0">
-        <v>0.2359322879500001</v>
+        <v>-0.061905877349999971</v>
       </c>
       <c r="F52" s="0">
-        <v>0.22426425521999999</v>
+        <v>0.0078527945049999964</v>
       </c>
       <c r="G52" s="0">
-        <v>0.43424018704</v>
+        <v>0.44272748997</v>
       </c>
       <c r="H52" s="0">
-        <v>0.18463068574499999</v>
+        <v>0.50785625629999998</v>
       </c>
       <c r="I52" s="0">
-        <v>0.0095842030000000134</v>
+        <v>0.072990685280000023</v>
       </c>
       <c r="J52" s="0">
-        <v>0.031173121599999964</v>
+        <v>-0.0087658969499999906</v>
       </c>
       <c r="K52" s="0">
-        <v>1.1859677202500001</v>
+        <v>1.33047208465</v>
       </c>
       <c r="L52" s="0">
-        <v>-0.044081079235000015</v>
+        <v>0.0046093837800000158</v>
       </c>
       <c r="M52" s="0">
-        <v>-2.2463942788</v>
+        <v>-2.0410842904500002</v>
       </c>
       <c r="N52" s="0">
-        <v>0.62863754524999993</v>
+        <v>-0.13956971094000006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>